<commit_message>
Complete analysis for lab1
</commit_message>
<xml_diff>
--- a/bmes301/lab1/data/lab1_test_data.xlsx
+++ b/bmes301/lab1/data/lab1_test_data.xlsx
@@ -446,12 +446,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>E (MPa)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>k (N/mm)</t>
         </is>
       </c>
     </row>
@@ -466,14 +466,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>02</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>12.11483330268918</v>
+        <v>4.833454170321591</v>
       </c>
       <c r="E2" t="n">
-        <v>4.330408499684641</v>
+        <v>1.325462690005715</v>
       </c>
     </row>
     <row r="3">
@@ -482,19 +482,19 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>LCL</t>
+          <t>MCL</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>08</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4.833454170321591</v>
+        <v>8.612915666753445</v>
       </c>
       <c r="E3" t="n">
-        <v>1.325462690005715</v>
+        <v>2.351042034748962</v>
       </c>
     </row>
     <row r="4">
@@ -508,14 +508,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>08</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>13.32303589345438</v>
+        <v>10.22701617502049</v>
       </c>
       <c r="E4" t="n">
-        <v>4.946177075444941</v>
+        <v>1.363602156669399</v>
       </c>
     </row>
     <row r="5">
@@ -524,19 +524,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LCL</t>
+          <t>MCL</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>05</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>21.07680203522363</v>
+        <v>20.04660225334274</v>
       </c>
       <c r="E5" t="n">
-        <v>2.965673914690758</v>
+        <v>4.747879481054859</v>
       </c>
     </row>
     <row r="6">
@@ -545,19 +545,19 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>LCL</t>
+          <t>MCL</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>04</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>31.7608406328724</v>
+        <v>17.60619541581704</v>
       </c>
       <c r="E6" t="n">
-        <v>4.466368213997681</v>
+        <v>5.711278025130895</v>
       </c>
     </row>
     <row r="7">
@@ -571,14 +571,14 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2.264103576822557</v>
+        <v>19.89518258065792</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3069970951623806</v>
+        <v>4.50456964090368</v>
       </c>
     </row>
     <row r="8">
@@ -587,19 +587,19 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>LCL</t>
+          <t>MCL</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>09</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>9.168396981614865</v>
+        <v>21.75123279164934</v>
       </c>
       <c r="E8" t="n">
-        <v>1.384132189482502</v>
+        <v>4.857775323468353</v>
       </c>
     </row>
     <row r="9">
@@ -608,19 +608,19 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LCL</t>
+          <t>MCL</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>10.22701617502049</v>
+        <v>9.433230463407448</v>
       </c>
       <c r="E9" t="n">
-        <v>1.363602156669399</v>
+        <v>3.074534373258724</v>
       </c>
     </row>
     <row r="10">
@@ -634,14 +634,14 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>04</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>10.8491727760429</v>
+        <v>21.07680203522363</v>
       </c>
       <c r="E10" t="n">
-        <v>2.608770553017949</v>
+        <v>2.965673914690758</v>
       </c>
     </row>
     <row r="11">
@@ -655,14 +655,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>03</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>19.89518258065792</v>
+        <v>13.32303589345438</v>
       </c>
       <c r="E11" t="n">
-        <v>4.50456964090368</v>
+        <v>4.946177075444941</v>
       </c>
     </row>
     <row r="12">
@@ -676,14 +676,14 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>07</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2.378275167186548</v>
+        <v>23.92605810181052</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9409697400607646</v>
+        <v>5.638021612109806</v>
       </c>
     </row>
     <row r="13">
@@ -692,19 +692,19 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MCL</t>
+          <t>LCL</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3.510014164356793</v>
+        <v>12.11483330268918</v>
       </c>
       <c r="E13" t="n">
-        <v>1.864159961679736</v>
+        <v>4.330408499684641</v>
       </c>
     </row>
     <row r="14">
@@ -718,14 +718,14 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>02</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>12.41061955319874</v>
+        <v>3.510014164356793</v>
       </c>
       <c r="E14" t="n">
-        <v>8.211409923554783</v>
+        <v>1.864159961679736</v>
       </c>
     </row>
     <row r="15">
@@ -739,14 +739,14 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>06</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>17.60619541581704</v>
+        <v>32.40808937901795</v>
       </c>
       <c r="E15" t="n">
-        <v>5.711278025130895</v>
+        <v>6.328105873481926</v>
       </c>
     </row>
     <row r="16">
@@ -755,7 +755,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MCL</t>
+          <t>LCL</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -764,10 +764,10 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>20.04660225334274</v>
+        <v>31.7608406328724</v>
       </c>
       <c r="E16" t="n">
-        <v>4.747879481054859</v>
+        <v>4.466368213997681</v>
       </c>
     </row>
     <row r="17">
@@ -781,14 +781,14 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>01</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>32.40808937901795</v>
+        <v>2.378275167186548</v>
       </c>
       <c r="E17" t="n">
-        <v>6.328105873481926</v>
+        <v>0.9409697400607646</v>
       </c>
     </row>
     <row r="18">
@@ -797,19 +797,19 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MCL</t>
+          <t>LCL</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>09</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>23.92605810181052</v>
+        <v>10.8491727760429</v>
       </c>
       <c r="E18" t="n">
-        <v>5.638021612109806</v>
+        <v>2.608770553017949</v>
       </c>
     </row>
     <row r="19">
@@ -823,14 +823,14 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>03</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>8.612915666753445</v>
+        <v>12.41061955319874</v>
       </c>
       <c r="E19" t="n">
-        <v>2.351042034748962</v>
+        <v>8.211409923554783</v>
       </c>
     </row>
     <row r="20">
@@ -839,19 +839,19 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MCL</t>
+          <t>LCL</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>06</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>21.75123279164934</v>
+        <v>2.264103576822557</v>
       </c>
       <c r="E20" t="n">
-        <v>4.857775323468353</v>
+        <v>0.3069970951623806</v>
       </c>
     </row>
     <row r="21">
@@ -860,19 +860,19 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>MCL</t>
+          <t>LCL</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>07</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>9.433230463407448</v>
+        <v>9.168396981614865</v>
       </c>
       <c r="E21" t="n">
-        <v>3.074534373258724</v>
+        <v>1.384132189482502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>